<commit_message>
test: tests for independent and collaborative strategies
</commit_message>
<xml_diff>
--- a/powersimdata/scaling/clean_capacity_scaling/Capacity_Scaling_Western_Test_Case.xlsx
+++ b/powersimdata/scaling/clean_capacity_scaling/Capacity_Scaling_Western_Test_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmuldrew\GitHub\PowerSimData\powersimdata\scaling\clean_capacity_scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DD7153-F10F-4431-98FD-9C3EBAE9B910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3FC454-478D-4DC9-B5F7-E811F5905DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30210" yWindow="3945" windowWidth="20925" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacity_Scaling_Western_Test_C" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t>State</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>El Paso</t>
-  </si>
-  <si>
-    <t>Western</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH14"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,32 +2397,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="S14">
-        <v>0.231050426</v>
-      </c>
-      <c r="T14">
-        <v>0.33124165999999999</v>
-      </c>
-      <c r="U14">
-        <v>0.231050426</v>
-      </c>
-      <c r="V14">
-        <v>0.33124165999999999</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <v>0.438</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: added additional next capacity functions to replicate previous results
</commit_message>
<xml_diff>
--- a/powersimdata/scaling/clean_capacity_scaling/Capacity_Scaling_Western_Test_Case.xlsx
+++ b/powersimdata/scaling/clean_capacity_scaling/Capacity_Scaling_Western_Test_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmuldrew\GitHub\PowerSimData\powersimdata\scaling\clean_capacity_scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3FC454-478D-4DC9-B5F7-E811F5905DB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24DE1F6-8913-4FE1-82B3-A582BD4C3797}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="6225" windowWidth="50535" windowHeight="11940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capacity_Scaling_Western_Test_C" sheetId="1" r:id="rId1"/>
@@ -1007,7 +1007,7 @@
   <dimension ref="A1:AH13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1229,7 @@
         <v>0.85799999999999998</v>
       </c>
       <c r="Z2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA2" t="s">
         <v>35</v>
@@ -1437,7 +1437,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="Z4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA4" t="s">
         <v>35</v>
@@ -1541,7 +1541,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="Z5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA5" t="s">
         <v>35</v>
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="Z6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA6" t="s">
         <v>35</v>
@@ -1749,7 +1749,7 @@
         <v>0.87</v>
       </c>
       <c r="Z7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA7" t="s">
         <v>35</v>
@@ -1853,7 +1853,7 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="Z8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA8" t="s">
         <v>35</v>
@@ -1957,7 +1957,7 @@
         <v>0.02</v>
       </c>
       <c r="Z9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA9" t="s">
         <v>35</v>
@@ -2061,7 +2061,7 @@
         <v>0.57899999999999996</v>
       </c>
       <c r="Z10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA10" t="s">
         <v>35</v>
@@ -2165,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA11" t="s">
         <v>36</v>
@@ -2269,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="Z12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA12" t="s">
         <v>35</v>
@@ -2355,13 +2355,13 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>0.34548755599999997</v>
       </c>
       <c r="U13">
         <v>0</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>0.34548755599999997</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -2369,8 +2369,11 @@
       <c r="X13">
         <v>0</v>
       </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
       <c r="Z13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA13" t="s">
         <v>35</v>

</xml_diff>